<commit_message>
updated comments in networks.py
</commit_message>
<xml_diff>
--- a/Documentation/ProjectGanttChart.xlsx
+++ b/Documentation/ProjectGanttChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cabb659577f8f2a6/Documents/UCF/Graduate Studies/Fall 2025/CAP 5415/Course Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cabb659577f8f2a6/Documents/UCF/Graduate Studies/Fall 2025/CAP 5415/Course Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{BC6BBFCB-F0CB-48F7-8EAB-1BA0930503B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D66CBDAC-27FF-4613-AFBA-57D4E62E9F82}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{BC6BBFCB-F0CB-48F7-8EAB-1BA0930503B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057668F6-5582-4573-88CE-E0BE57D77EF3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,22 +1019,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1046,14 +1043,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1658,28 +1658,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="106" t="s">
+      <c r="I1" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="105">
+      <c r="Q1" s="104">
         <v>45986</v>
       </c>
-      <c r="R1" s="104"/>
-      <c r="S1" s="104"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
-      <c r="Y1" s="104"/>
-      <c r="Z1" s="104"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B2" s="82"/>
@@ -1689,28 +1689,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="103">
+      <c r="Q2" s="102">
         <v>1</v>
       </c>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="104"/>
-      <c r="V2" s="104"/>
-      <c r="W2" s="104"/>
-      <c r="X2" s="104"/>
-      <c r="Y2" s="104"/>
-      <c r="Z2" s="104"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
@@ -1726,102 +1726,102 @@
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="110">
+      <c r="I4" s="99">
         <f>I5</f>
         <v>45985</v>
       </c>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108">
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97">
         <f>P5</f>
         <v>45992</v>
       </c>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="108">
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97">
         <f>W5</f>
         <v>45999</v>
       </c>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="108"/>
-      <c r="AB4" s="108"/>
-      <c r="AC4" s="108"/>
-      <c r="AD4" s="108">
+      <c r="X4" s="97"/>
+      <c r="Y4" s="97"/>
+      <c r="Z4" s="97"/>
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97">
         <f>AD5</f>
         <v>46006</v>
       </c>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="108"/>
-      <c r="AH4" s="108"/>
-      <c r="AI4" s="108"/>
-      <c r="AJ4" s="108"/>
-      <c r="AK4" s="108">
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="97"/>
+      <c r="AG4" s="97"/>
+      <c r="AH4" s="97"/>
+      <c r="AI4" s="97"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="97">
         <f>AK5</f>
         <v>46013</v>
       </c>
-      <c r="AL4" s="108"/>
-      <c r="AM4" s="108"/>
-      <c r="AN4" s="108"/>
-      <c r="AO4" s="108"/>
-      <c r="AP4" s="108"/>
-      <c r="AQ4" s="108"/>
-      <c r="AR4" s="108">
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="97"/>
+      <c r="AN4" s="97"/>
+      <c r="AO4" s="97"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="97"/>
+      <c r="AR4" s="97">
         <f>AR5</f>
         <v>46020</v>
       </c>
-      <c r="AS4" s="108"/>
-      <c r="AT4" s="108"/>
-      <c r="AU4" s="108"/>
-      <c r="AV4" s="108"/>
-      <c r="AW4" s="108"/>
-      <c r="AX4" s="108"/>
-      <c r="AY4" s="108">
+      <c r="AS4" s="97"/>
+      <c r="AT4" s="97"/>
+      <c r="AU4" s="97"/>
+      <c r="AV4" s="97"/>
+      <c r="AW4" s="97"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="97">
         <f>AY5</f>
         <v>46027</v>
       </c>
-      <c r="AZ4" s="108"/>
-      <c r="BA4" s="108"/>
-      <c r="BB4" s="108"/>
-      <c r="BC4" s="108"/>
-      <c r="BD4" s="108"/>
-      <c r="BE4" s="108"/>
-      <c r="BF4" s="108">
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="97"/>
+      <c r="BB4" s="97"/>
+      <c r="BC4" s="97"/>
+      <c r="BD4" s="97"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="97">
         <f>BF5</f>
         <v>46034</v>
       </c>
-      <c r="BG4" s="108"/>
-      <c r="BH4" s="108"/>
-      <c r="BI4" s="108"/>
-      <c r="BJ4" s="108"/>
-      <c r="BK4" s="108"/>
-      <c r="BL4" s="109"/>
+      <c r="BG4" s="97"/>
+      <c r="BH4" s="97"/>
+      <c r="BI4" s="97"/>
+      <c r="BJ4" s="97"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="98"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="97"/>
-      <c r="B5" s="98" t="s">
+      <c r="A5" s="107"/>
+      <c r="B5" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="102" t="s">
+      <c r="D5" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="102" t="s">
+      <c r="F5" s="100" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2050,8 +2050,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="97"/>
-      <c r="B6" s="99"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="101"/>
       <c r="D6" s="101"/>
       <c r="E6" s="101"/>
@@ -3462,7 +3462,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="94">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="E22" s="95">
         <v>45994</v>
@@ -3626,6 +3626,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -3634,16 +3644,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D24">
     <cfRule type="dataBar" priority="23">
@@ -3882,15 +3882,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4202,6 +4193,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -4222,14 +4222,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4250,6 +4242,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
updated readme and comments on generator.py
</commit_message>
<xml_diff>
--- a/Documentation/ProjectGanttChart.xlsx
+++ b/Documentation/ProjectGanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cabb659577f8f2a6/Documents/UCF/Graduate Studies/Fall 2025/CAP 5415/Course Project/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cabb659577f8f2a6/Documents/UCF/Graduate Studies/Fall 2025/CAP 5415/Course Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{BC6BBFCB-F0CB-48F7-8EAB-1BA0930503B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{057668F6-5582-4573-88CE-E0BE57D77EF3}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{BC6BBFCB-F0CB-48F7-8EAB-1BA0930503B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4561088D-98E4-6E4E-BFAE-D245B8351E75}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="task_start" localSheetId="0">'Project schedule'!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -482,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -720,6 +720,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -751,7 +775,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -863,9 +887,6 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -899,9 +920,6 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1003,21 +1021,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="19" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1053,6 +1056,42 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1629,28 +1668,28 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL27"/>
+  <dimension ref="A1:BM27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B14" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="7" width="2.75" customWidth="1"/>
-    <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="65" width="2.75" customWidth="1"/>
+    <col min="1" max="1" width="2.6953125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="26.48046875" customWidth="1"/>
+    <col min="3" max="3" width="16.671875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.6953125" customWidth="1"/>
+    <col min="8" max="8" width="6.00390625" hidden="1" customWidth="1"/>
+    <col min="9" max="65" width="2.6953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="2.25">
+    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A1" s="14"/>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="82" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="18"/>
@@ -1658,61 +1697,61 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="105" t="s">
+      <c r="I1" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="104">
+      <c r="Q1" s="97">
         <v>45986</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="103"/>
-      <c r="W1" s="103"/>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="82"/>
-      <c r="C2" s="83" t="s">
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="80"/>
+      <c r="C2" s="81" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="102">
+      <c r="Q2" s="95">
         <v>1</v>
       </c>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="103"/>
-    </row>
-    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+    </row>
+    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="13"/>
       <c r="B3" s="25" t="s">
         <v>8</v>
@@ -1720,108 +1759,108 @@
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14"/>
       <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="99">
+      <c r="I4" s="92">
         <f>I5</f>
         <v>45985</v>
       </c>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="97">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90">
         <f>P5</f>
         <v>45992</v>
       </c>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="97">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90">
         <f>W5</f>
         <v>45999</v>
       </c>
-      <c r="X4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="90">
         <f>AD5</f>
         <v>46006</v>
       </c>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="97">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="90">
         <f>AK5</f>
         <v>46013</v>
       </c>
-      <c r="AL4" s="97"/>
-      <c r="AM4" s="97"/>
-      <c r="AN4" s="97"/>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="97">
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="90">
         <f>AR5</f>
         <v>46020</v>
       </c>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="97"/>
-      <c r="AU4" s="97"/>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="97">
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="90">
         <f>AY5</f>
         <v>46027</v>
       </c>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="97"/>
-      <c r="BB4" s="97"/>
-      <c r="BC4" s="97"/>
-      <c r="BD4" s="97"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="97">
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="90">
         <f>BF5</f>
         <v>46034</v>
       </c>
-      <c r="BG4" s="97"/>
-      <c r="BH4" s="97"/>
-      <c r="BI4" s="97"/>
-      <c r="BJ4" s="97"/>
-      <c r="BK4" s="97"/>
-      <c r="BL4" s="98"/>
-    </row>
-    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108" t="s">
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
+    </row>
+    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="100"/>
+      <c r="B5" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="100" t="s">
+      <c r="D5" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="100" t="s">
+      <c r="E5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="100" t="s">
+      <c r="F5" s="93" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2049,13 +2088,13 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="107"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="100"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
       <c r="I6" s="34" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2281,7 +2320,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -2291,7 +2330,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="H7" s="26" t="str">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="39"/>
@@ -2351,7 +2390,7 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
         <v>22</v>
@@ -2362,1266 +2401,1323 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H24" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H24" ca="1" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="45"/>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="45"/>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="45"/>
-      <c r="AG8" s="45"/>
-      <c r="AH8" s="45"/>
-      <c r="AI8" s="45"/>
-      <c r="AJ8" s="45"/>
-      <c r="AK8" s="45"/>
-      <c r="AL8" s="45"/>
-      <c r="AM8" s="45"/>
-      <c r="AN8" s="45"/>
-      <c r="AO8" s="45"/>
-      <c r="AP8" s="45"/>
-      <c r="AQ8" s="45"/>
-      <c r="AR8" s="45"/>
-      <c r="AS8" s="45"/>
-      <c r="AT8" s="45"/>
-      <c r="AU8" s="45"/>
-      <c r="AV8" s="45"/>
-      <c r="AW8" s="45"/>
-      <c r="AX8" s="45"/>
-      <c r="AY8" s="45"/>
-      <c r="AZ8" s="45"/>
-      <c r="BA8" s="45"/>
-      <c r="BB8" s="45"/>
-      <c r="BC8" s="45"/>
-      <c r="BD8" s="45"/>
-      <c r="BE8" s="45"/>
-      <c r="BF8" s="45"/>
-      <c r="BG8" s="45"/>
-      <c r="BH8" s="45"/>
-      <c r="BI8" s="45"/>
-      <c r="BJ8" s="45"/>
-      <c r="BK8" s="45"/>
-      <c r="BL8" s="45"/>
-    </row>
-    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="108"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="108"/>
+      <c r="U8" s="108"/>
+      <c r="V8" s="108"/>
+      <c r="W8" s="108"/>
+      <c r="X8" s="108"/>
+      <c r="Y8" s="108"/>
+      <c r="Z8" s="108"/>
+      <c r="AA8" s="108"/>
+      <c r="AB8" s="108"/>
+      <c r="AC8" s="108"/>
+      <c r="AD8" s="108"/>
+      <c r="AE8" s="108"/>
+      <c r="AF8" s="108"/>
+      <c r="AG8" s="108"/>
+      <c r="AH8" s="108"/>
+      <c r="AI8" s="108"/>
+      <c r="AJ8" s="108"/>
+      <c r="AK8" s="108"/>
+      <c r="AL8" s="108"/>
+      <c r="AM8" s="108"/>
+      <c r="AN8" s="108"/>
+      <c r="AO8" s="108"/>
+      <c r="AP8" s="108"/>
+      <c r="AQ8" s="108"/>
+      <c r="AR8" s="108"/>
+      <c r="AS8" s="108"/>
+      <c r="AT8" s="108"/>
+      <c r="AU8" s="108"/>
+      <c r="AV8" s="108"/>
+      <c r="AW8" s="108"/>
+      <c r="AX8" s="108"/>
+      <c r="AY8" s="108"/>
+      <c r="AZ8" s="108"/>
+      <c r="BA8" s="108"/>
+      <c r="BB8" s="108"/>
+      <c r="BC8" s="108"/>
+      <c r="BD8" s="108"/>
+      <c r="BE8" s="108"/>
+      <c r="BF8" s="108"/>
+      <c r="BG8" s="108"/>
+      <c r="BH8" s="108"/>
+      <c r="BI8" s="108"/>
+      <c r="BJ8" s="108"/>
+      <c r="BK8" s="108"/>
+      <c r="BL8" s="108"/>
+    </row>
+    <row r="9" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>1</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="49">
         <f>Project_Start</f>
         <v>45986</v>
       </c>
-      <c r="F9" s="50">
+      <c r="F9" s="49">
         <f>E9+1</f>
         <v>45987</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="51"/>
-      <c r="T9" s="51"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
-      <c r="X9" s="51"/>
-      <c r="Y9" s="51"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="51"/>
-      <c r="AB9" s="51"/>
-      <c r="AC9" s="51"/>
-      <c r="AD9" s="51"/>
-      <c r="AE9" s="51"/>
-      <c r="AF9" s="51"/>
-      <c r="AG9" s="51"/>
-      <c r="AH9" s="51"/>
-      <c r="AI9" s="51"/>
-      <c r="AJ9" s="51"/>
-      <c r="AK9" s="51"/>
-      <c r="AL9" s="51"/>
-      <c r="AM9" s="51"/>
-      <c r="AN9" s="51"/>
-      <c r="AO9" s="51"/>
-      <c r="AP9" s="51"/>
-      <c r="AQ9" s="51"/>
-      <c r="AR9" s="51"/>
-      <c r="AS9" s="51"/>
-      <c r="AT9" s="51"/>
-      <c r="AU9" s="51"/>
-      <c r="AV9" s="51"/>
-      <c r="AW9" s="51"/>
-      <c r="AX9" s="51"/>
-      <c r="AY9" s="51"/>
-      <c r="AZ9" s="51"/>
-      <c r="BA9" s="51"/>
-      <c r="BB9" s="51"/>
-      <c r="BC9" s="51"/>
-      <c r="BD9" s="51"/>
-      <c r="BE9" s="51"/>
-      <c r="BF9" s="51"/>
-      <c r="BG9" s="51"/>
-      <c r="BH9" s="51"/>
-      <c r="BI9" s="51"/>
-      <c r="BJ9" s="51"/>
-      <c r="BK9" s="51"/>
-      <c r="BL9" s="51"/>
-    </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114"/>
+      <c r="R9" s="114"/>
+      <c r="S9" s="114"/>
+      <c r="T9" s="114"/>
+      <c r="U9" s="114"/>
+      <c r="V9" s="114"/>
+      <c r="W9" s="114"/>
+      <c r="X9" s="114"/>
+      <c r="Y9" s="114"/>
+      <c r="Z9" s="114"/>
+      <c r="AA9" s="114"/>
+      <c r="AB9" s="114"/>
+      <c r="AC9" s="114"/>
+      <c r="AD9" s="114"/>
+      <c r="AE9" s="114"/>
+      <c r="AF9" s="114"/>
+      <c r="AG9" s="114"/>
+      <c r="AH9" s="114"/>
+      <c r="AI9" s="114"/>
+      <c r="AJ9" s="114"/>
+      <c r="AK9" s="114"/>
+      <c r="AL9" s="114"/>
+      <c r="AM9" s="114"/>
+      <c r="AN9" s="114"/>
+      <c r="AO9" s="114"/>
+      <c r="AP9" s="114"/>
+      <c r="AQ9" s="114"/>
+      <c r="AR9" s="114"/>
+      <c r="AS9" s="114"/>
+      <c r="AT9" s="114"/>
+      <c r="AU9" s="114"/>
+      <c r="AV9" s="114"/>
+      <c r="AW9" s="114"/>
+      <c r="AX9" s="114"/>
+      <c r="AY9" s="114"/>
+      <c r="AZ9" s="114"/>
+      <c r="BA9" s="114"/>
+      <c r="BB9" s="114"/>
+      <c r="BC9" s="114"/>
+      <c r="BD9" s="114"/>
+      <c r="BE9" s="114"/>
+      <c r="BF9" s="114"/>
+      <c r="BG9" s="114"/>
+      <c r="BH9" s="114"/>
+      <c r="BI9" s="114"/>
+      <c r="BJ9" s="114"/>
+      <c r="BK9" s="114"/>
+      <c r="BL9" s="114"/>
+    </row>
+    <row r="10" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="17"/>
       <c r="H10" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="57"/>
-      <c r="AA10" s="57"/>
-      <c r="AB10" s="57"/>
-      <c r="AC10" s="57"/>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="57"/>
-      <c r="AF10" s="57"/>
-      <c r="AG10" s="57"/>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="57"/>
-      <c r="AJ10" s="57"/>
-      <c r="AK10" s="57"/>
-      <c r="AL10" s="57"/>
-      <c r="AM10" s="57"/>
-      <c r="AN10" s="57"/>
-      <c r="AO10" s="57"/>
-      <c r="AP10" s="57"/>
-      <c r="AQ10" s="57"/>
-      <c r="AR10" s="57"/>
-      <c r="AS10" s="57"/>
-      <c r="AT10" s="57"/>
-      <c r="AU10" s="57"/>
-      <c r="AV10" s="57"/>
-      <c r="AW10" s="57"/>
-      <c r="AX10" s="57"/>
-      <c r="AY10" s="57"/>
-      <c r="AZ10" s="57"/>
-      <c r="BA10" s="57"/>
-      <c r="BB10" s="57"/>
-      <c r="BC10" s="57"/>
-      <c r="BD10" s="57"/>
-      <c r="BE10" s="57"/>
-      <c r="BF10" s="57"/>
-      <c r="BG10" s="57"/>
-      <c r="BH10" s="57"/>
-      <c r="BI10" s="57"/>
-      <c r="BJ10" s="57"/>
-      <c r="BK10" s="57"/>
-      <c r="BL10" s="57"/>
-    </row>
-    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="115"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="115"/>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="115"/>
+      <c r="R10" s="115"/>
+      <c r="S10" s="115"/>
+      <c r="T10" s="115"/>
+      <c r="U10" s="115"/>
+      <c r="V10" s="115"/>
+      <c r="W10" s="115"/>
+      <c r="X10" s="115"/>
+      <c r="Y10" s="115"/>
+      <c r="Z10" s="115"/>
+      <c r="AA10" s="115"/>
+      <c r="AB10" s="115"/>
+      <c r="AC10" s="115"/>
+      <c r="AD10" s="115"/>
+      <c r="AE10" s="115"/>
+      <c r="AF10" s="115"/>
+      <c r="AG10" s="115"/>
+      <c r="AH10" s="115"/>
+      <c r="AI10" s="115"/>
+      <c r="AJ10" s="115"/>
+      <c r="AK10" s="115"/>
+      <c r="AL10" s="115"/>
+      <c r="AM10" s="115"/>
+      <c r="AN10" s="115"/>
+      <c r="AO10" s="115"/>
+      <c r="AP10" s="115"/>
+      <c r="AQ10" s="115"/>
+      <c r="AR10" s="115"/>
+      <c r="AS10" s="115"/>
+      <c r="AT10" s="115"/>
+      <c r="AU10" s="115"/>
+      <c r="AV10" s="115"/>
+      <c r="AW10" s="115"/>
+      <c r="AX10" s="115"/>
+      <c r="AY10" s="115"/>
+      <c r="AZ10" s="115"/>
+      <c r="BA10" s="115"/>
+      <c r="BB10" s="115"/>
+      <c r="BC10" s="115"/>
+      <c r="BD10" s="115"/>
+      <c r="BE10" s="115"/>
+      <c r="BF10" s="115"/>
+      <c r="BG10" s="115"/>
+      <c r="BH10" s="115"/>
+      <c r="BI10" s="115"/>
+      <c r="BJ10" s="115"/>
+      <c r="BK10" s="115"/>
+      <c r="BL10" s="115"/>
+    </row>
+    <row r="11" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="58">
         <v>1</v>
       </c>
-      <c r="E11" s="61">
+      <c r="E11" s="59">
         <v>45986</v>
       </c>
-      <c r="F11" s="61">
+      <c r="F11" s="59">
         <f>E11+1</f>
         <v>45987</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="51"/>
-      <c r="W11" s="51"/>
-      <c r="X11" s="51"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="51"/>
-      <c r="AA11" s="51"/>
-      <c r="AB11" s="51"/>
-      <c r="AC11" s="51"/>
-      <c r="AD11" s="51"/>
-      <c r="AE11" s="51"/>
-      <c r="AF11" s="51"/>
-      <c r="AG11" s="51"/>
-      <c r="AH11" s="51"/>
-      <c r="AI11" s="51"/>
-      <c r="AJ11" s="51"/>
-      <c r="AK11" s="51"/>
-      <c r="AL11" s="51"/>
-      <c r="AM11" s="51"/>
-      <c r="AN11" s="51"/>
-      <c r="AO11" s="51"/>
-      <c r="AP11" s="51"/>
-      <c r="AQ11" s="51"/>
-      <c r="AR11" s="51"/>
-      <c r="AS11" s="51"/>
-      <c r="AT11" s="51"/>
-      <c r="AU11" s="51"/>
-      <c r="AV11" s="51"/>
-      <c r="AW11" s="51"/>
-      <c r="AX11" s="51"/>
-      <c r="AY11" s="51"/>
-      <c r="AZ11" s="51"/>
-      <c r="BA11" s="51"/>
-      <c r="BB11" s="51"/>
-      <c r="BC11" s="51"/>
-      <c r="BD11" s="51"/>
-      <c r="BE11" s="51"/>
-      <c r="BF11" s="51"/>
-      <c r="BG11" s="51"/>
-      <c r="BH11" s="51"/>
-      <c r="BI11" s="51"/>
-      <c r="BJ11" s="51"/>
-      <c r="BK11" s="51"/>
-      <c r="BL11" s="51"/>
-    </row>
-    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="113"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="113"/>
+      <c r="R11" s="113"/>
+      <c r="S11" s="113"/>
+      <c r="T11" s="113"/>
+      <c r="U11" s="113"/>
+      <c r="V11" s="113"/>
+      <c r="W11" s="113"/>
+      <c r="X11" s="113"/>
+      <c r="Y11" s="113"/>
+      <c r="Z11" s="113"/>
+      <c r="AA11" s="113"/>
+      <c r="AB11" s="113"/>
+      <c r="AC11" s="113"/>
+      <c r="AD11" s="113"/>
+      <c r="AE11" s="113"/>
+      <c r="AF11" s="113"/>
+      <c r="AG11" s="113"/>
+      <c r="AH11" s="113"/>
+      <c r="AI11" s="113"/>
+      <c r="AJ11" s="113"/>
+      <c r="AK11" s="113"/>
+      <c r="AL11" s="113"/>
+      <c r="AM11" s="113"/>
+      <c r="AN11" s="113"/>
+      <c r="AO11" s="113"/>
+      <c r="AP11" s="113"/>
+      <c r="AQ11" s="113"/>
+      <c r="AR11" s="113"/>
+      <c r="AS11" s="113"/>
+      <c r="AT11" s="113"/>
+      <c r="AU11" s="113"/>
+      <c r="AV11" s="113"/>
+      <c r="AW11" s="113"/>
+      <c r="AX11" s="113"/>
+      <c r="AY11" s="113"/>
+      <c r="AZ11" s="113"/>
+      <c r="BA11" s="113"/>
+      <c r="BB11" s="113"/>
+      <c r="BC11" s="113"/>
+      <c r="BD11" s="113"/>
+      <c r="BE11" s="113"/>
+      <c r="BF11" s="113"/>
+      <c r="BG11" s="113"/>
+      <c r="BH11" s="113"/>
+      <c r="BI11" s="113"/>
+      <c r="BJ11" s="113"/>
+      <c r="BK11" s="113"/>
+      <c r="BL11" s="113"/>
+    </row>
+    <row r="12" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="58">
         <v>1</v>
       </c>
-      <c r="E12" s="61">
+      <c r="E12" s="59">
         <f>F11+1</f>
         <v>45988</v>
       </c>
-      <c r="F12" s="61">
+      <c r="F12" s="59">
         <f>E12+1</f>
         <v>45989</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="51"/>
-      <c r="AB12" s="51"/>
-      <c r="AC12" s="51"/>
-      <c r="AD12" s="51"/>
-      <c r="AE12" s="51"/>
-      <c r="AF12" s="51"/>
-      <c r="AG12" s="51"/>
-      <c r="AH12" s="51"/>
-      <c r="AI12" s="51"/>
-      <c r="AJ12" s="51"/>
-      <c r="AK12" s="51"/>
-      <c r="AL12" s="51"/>
-      <c r="AM12" s="51"/>
-      <c r="AN12" s="51"/>
-      <c r="AO12" s="51"/>
-      <c r="AP12" s="51"/>
-      <c r="AQ12" s="51"/>
-      <c r="AR12" s="51"/>
-      <c r="AS12" s="51"/>
-      <c r="AT12" s="51"/>
-      <c r="AU12" s="51"/>
-      <c r="AV12" s="51"/>
-      <c r="AW12" s="51"/>
-      <c r="AX12" s="51"/>
-      <c r="AY12" s="51"/>
-      <c r="AZ12" s="51"/>
-      <c r="BA12" s="51"/>
-      <c r="BB12" s="51"/>
-      <c r="BC12" s="51"/>
-      <c r="BD12" s="51"/>
-      <c r="BE12" s="51"/>
-      <c r="BF12" s="51"/>
-      <c r="BG12" s="51"/>
-      <c r="BH12" s="51"/>
-      <c r="BI12" s="51"/>
-      <c r="BJ12" s="51"/>
-      <c r="BK12" s="51"/>
-      <c r="BL12" s="51"/>
-    </row>
-    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
+      <c r="AC12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50"/>
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="50"/>
+      <c r="AM12" s="50"/>
+      <c r="AN12" s="50"/>
+      <c r="AO12" s="50"/>
+      <c r="AP12" s="50"/>
+      <c r="AQ12" s="50"/>
+      <c r="AR12" s="50"/>
+      <c r="AS12" s="50"/>
+      <c r="AT12" s="50"/>
+      <c r="AU12" s="50"/>
+      <c r="AV12" s="50"/>
+      <c r="AW12" s="50"/>
+      <c r="AX12" s="50"/>
+      <c r="AY12" s="50"/>
+      <c r="AZ12" s="50"/>
+      <c r="BA12" s="50"/>
+      <c r="BB12" s="50"/>
+      <c r="BC12" s="50"/>
+      <c r="BD12" s="50"/>
+      <c r="BE12" s="50"/>
+      <c r="BF12" s="50"/>
+      <c r="BG12" s="50"/>
+      <c r="BH12" s="50"/>
+      <c r="BI12" s="50"/>
+      <c r="BJ12" s="50"/>
+      <c r="BK12" s="50"/>
+      <c r="BL12" s="50"/>
+    </row>
+    <row r="13" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="60">
+      <c r="D13" s="58">
         <v>1</v>
       </c>
-      <c r="E13" s="61">
+      <c r="E13" s="59">
         <f>E12+1</f>
         <v>45989</v>
       </c>
-      <c r="F13" s="61">
+      <c r="F13" s="59">
         <f>E13+1</f>
         <v>45990</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="51"/>
-      <c r="AC13" s="51"/>
-      <c r="AD13" s="51"/>
-      <c r="AE13" s="51"/>
-      <c r="AF13" s="51"/>
-      <c r="AG13" s="51"/>
-      <c r="AH13" s="51"/>
-      <c r="AI13" s="51"/>
-      <c r="AJ13" s="51"/>
-      <c r="AK13" s="51"/>
-      <c r="AL13" s="51"/>
-      <c r="AM13" s="51"/>
-      <c r="AN13" s="51"/>
-      <c r="AO13" s="51"/>
-      <c r="AP13" s="51"/>
-      <c r="AQ13" s="51"/>
-      <c r="AR13" s="51"/>
-      <c r="AS13" s="51"/>
-      <c r="AT13" s="51"/>
-      <c r="AU13" s="51"/>
-      <c r="AV13" s="51"/>
-      <c r="AW13" s="51"/>
-      <c r="AX13" s="51"/>
-      <c r="AY13" s="51"/>
-      <c r="AZ13" s="51"/>
-      <c r="BA13" s="51"/>
-      <c r="BB13" s="51"/>
-      <c r="BC13" s="51"/>
-      <c r="BD13" s="51"/>
-      <c r="BE13" s="51"/>
-      <c r="BF13" s="51"/>
-      <c r="BG13" s="51"/>
-      <c r="BH13" s="51"/>
-      <c r="BI13" s="51"/>
-      <c r="BJ13" s="51"/>
-      <c r="BK13" s="51"/>
-      <c r="BL13" s="51"/>
-    </row>
-    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
+      <c r="AF13" s="50"/>
+      <c r="AG13" s="50"/>
+      <c r="AH13" s="50"/>
+      <c r="AI13" s="50"/>
+      <c r="AJ13" s="50"/>
+      <c r="AK13" s="50"/>
+      <c r="AL13" s="50"/>
+      <c r="AM13" s="50"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="50"/>
+      <c r="AP13" s="50"/>
+      <c r="AQ13" s="50"/>
+      <c r="AR13" s="50"/>
+      <c r="AS13" s="50"/>
+      <c r="AT13" s="50"/>
+      <c r="AU13" s="50"/>
+      <c r="AV13" s="50"/>
+      <c r="AW13" s="50"/>
+      <c r="AX13" s="50"/>
+      <c r="AY13" s="50"/>
+      <c r="AZ13" s="50"/>
+      <c r="BA13" s="50"/>
+      <c r="BB13" s="50"/>
+      <c r="BC13" s="50"/>
+      <c r="BD13" s="50"/>
+      <c r="BE13" s="50"/>
+      <c r="BF13" s="50"/>
+      <c r="BG13" s="50"/>
+      <c r="BH13" s="50"/>
+      <c r="BI13" s="50"/>
+      <c r="BJ13" s="50"/>
+      <c r="BK13" s="50"/>
+      <c r="BL13" s="50"/>
+    </row>
+    <row r="14" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="60">
+      <c r="D14" s="58">
         <v>1</v>
       </c>
-      <c r="E14" s="61">
+      <c r="E14" s="59">
         <f>E13</f>
         <v>45989</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="59">
         <f>E14+1</f>
         <v>45990</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="51"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="51"/>
-      <c r="AA14" s="51"/>
-      <c r="AB14" s="51"/>
-      <c r="AC14" s="51"/>
-      <c r="AD14" s="51"/>
-      <c r="AE14" s="51"/>
-      <c r="AF14" s="51"/>
-      <c r="AG14" s="51"/>
-      <c r="AH14" s="51"/>
-      <c r="AI14" s="51"/>
-      <c r="AJ14" s="51"/>
-      <c r="AK14" s="51"/>
-      <c r="AL14" s="51"/>
-      <c r="AM14" s="51"/>
-      <c r="AN14" s="51"/>
-      <c r="AO14" s="51"/>
-      <c r="AP14" s="51"/>
-      <c r="AQ14" s="51"/>
-      <c r="AR14" s="51"/>
-      <c r="AS14" s="51"/>
-      <c r="AT14" s="51"/>
-      <c r="AU14" s="51"/>
-      <c r="AV14" s="51"/>
-      <c r="AW14" s="51"/>
-      <c r="AX14" s="51"/>
-      <c r="AY14" s="51"/>
-      <c r="AZ14" s="51"/>
-      <c r="BA14" s="51"/>
-      <c r="BB14" s="51"/>
-      <c r="BC14" s="51"/>
-      <c r="BD14" s="51"/>
-      <c r="BE14" s="51"/>
-      <c r="BF14" s="51"/>
-      <c r="BG14" s="51"/>
-      <c r="BH14" s="51"/>
-      <c r="BI14" s="51"/>
-      <c r="BJ14" s="51"/>
-      <c r="BK14" s="51"/>
-      <c r="BL14" s="51"/>
-    </row>
-    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="50"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="50"/>
+      <c r="AC14" s="50"/>
+      <c r="AD14" s="50"/>
+      <c r="AE14" s="50"/>
+      <c r="AF14" s="50"/>
+      <c r="AG14" s="50"/>
+      <c r="AH14" s="50"/>
+      <c r="AI14" s="50"/>
+      <c r="AJ14" s="50"/>
+      <c r="AK14" s="50"/>
+      <c r="AL14" s="50"/>
+      <c r="AM14" s="50"/>
+      <c r="AN14" s="50"/>
+      <c r="AO14" s="50"/>
+      <c r="AP14" s="50"/>
+      <c r="AQ14" s="50"/>
+      <c r="AR14" s="50"/>
+      <c r="AS14" s="50"/>
+      <c r="AT14" s="50"/>
+      <c r="AU14" s="50"/>
+      <c r="AV14" s="50"/>
+      <c r="AW14" s="50"/>
+      <c r="AX14" s="50"/>
+      <c r="AY14" s="50"/>
+      <c r="AZ14" s="50"/>
+      <c r="BA14" s="50"/>
+      <c r="BB14" s="50"/>
+      <c r="BC14" s="50"/>
+      <c r="BD14" s="50"/>
+      <c r="BE14" s="50"/>
+      <c r="BF14" s="50"/>
+      <c r="BG14" s="50"/>
+      <c r="BH14" s="50"/>
+      <c r="BI14" s="50"/>
+      <c r="BJ14" s="50"/>
+      <c r="BK14" s="50"/>
+      <c r="BL14" s="50"/>
+    </row>
+    <row r="15" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="58">
         <v>1</v>
       </c>
-      <c r="E15" s="61">
+      <c r="E15" s="59">
         <f>F14+1</f>
         <v>45991</v>
       </c>
-      <c r="F15" s="61">
+      <c r="F15" s="59">
         <f>E15+2</f>
         <v>45993</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>3</v>
       </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="51"/>
-      <c r="Z15" s="51"/>
-      <c r="AA15" s="51"/>
-      <c r="AB15" s="51"/>
-      <c r="AC15" s="51"/>
-      <c r="AD15" s="51"/>
-      <c r="AE15" s="51"/>
-      <c r="AF15" s="51"/>
-      <c r="AG15" s="51"/>
-      <c r="AH15" s="51"/>
-      <c r="AI15" s="51"/>
-      <c r="AJ15" s="51"/>
-      <c r="AK15" s="51"/>
-      <c r="AL15" s="51"/>
-      <c r="AM15" s="51"/>
-      <c r="AN15" s="51"/>
-      <c r="AO15" s="51"/>
-      <c r="AP15" s="51"/>
-      <c r="AQ15" s="51"/>
-      <c r="AR15" s="51"/>
-      <c r="AS15" s="51"/>
-      <c r="AT15" s="51"/>
-      <c r="AU15" s="51"/>
-      <c r="AV15" s="51"/>
-      <c r="AW15" s="51"/>
-      <c r="AX15" s="51"/>
-      <c r="AY15" s="51"/>
-      <c r="AZ15" s="51"/>
-      <c r="BA15" s="51"/>
-      <c r="BB15" s="51"/>
-      <c r="BC15" s="51"/>
-      <c r="BD15" s="51"/>
-      <c r="BE15" s="51"/>
-      <c r="BF15" s="51"/>
-      <c r="BG15" s="51"/>
-      <c r="BH15" s="51"/>
-      <c r="BI15" s="51"/>
-      <c r="BJ15" s="51"/>
-      <c r="BK15" s="51"/>
-      <c r="BL15" s="51"/>
-    </row>
-    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="50"/>
+      <c r="Z15" s="50"/>
+      <c r="AA15" s="50"/>
+      <c r="AB15" s="50"/>
+      <c r="AC15" s="50"/>
+      <c r="AD15" s="50"/>
+      <c r="AE15" s="50"/>
+      <c r="AF15" s="50"/>
+      <c r="AG15" s="50"/>
+      <c r="AH15" s="50"/>
+      <c r="AI15" s="50"/>
+      <c r="AJ15" s="50"/>
+      <c r="AK15" s="50"/>
+      <c r="AL15" s="50"/>
+      <c r="AM15" s="50"/>
+      <c r="AN15" s="50"/>
+      <c r="AO15" s="50"/>
+      <c r="AP15" s="50"/>
+      <c r="AQ15" s="50"/>
+      <c r="AR15" s="50"/>
+      <c r="AS15" s="50"/>
+      <c r="AT15" s="50"/>
+      <c r="AU15" s="50"/>
+      <c r="AV15" s="50"/>
+      <c r="AW15" s="50"/>
+      <c r="AX15" s="50"/>
+      <c r="AY15" s="50"/>
+      <c r="AZ15" s="50"/>
+      <c r="BA15" s="50"/>
+      <c r="BB15" s="50"/>
+      <c r="BC15" s="50"/>
+      <c r="BD15" s="50"/>
+      <c r="BE15" s="50"/>
+      <c r="BF15" s="50"/>
+      <c r="BG15" s="50"/>
+      <c r="BH15" s="50"/>
+      <c r="BI15" s="50"/>
+      <c r="BJ15" s="50"/>
+      <c r="BK15" s="50"/>
+      <c r="BL15" s="50"/>
+    </row>
+    <row r="16" spans="1:64" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="17"/>
       <c r="H16" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="67"/>
-      <c r="R16" s="67"/>
-      <c r="S16" s="67"/>
-      <c r="T16" s="67"/>
-      <c r="U16" s="67"/>
-      <c r="V16" s="67"/>
-      <c r="W16" s="67"/>
-      <c r="X16" s="67"/>
-      <c r="Y16" s="67"/>
-      <c r="Z16" s="67"/>
-      <c r="AA16" s="67"/>
-      <c r="AB16" s="67"/>
-      <c r="AC16" s="67"/>
-      <c r="AD16" s="67"/>
-      <c r="AE16" s="67"/>
-      <c r="AF16" s="67"/>
-      <c r="AG16" s="67"/>
-      <c r="AH16" s="67"/>
-      <c r="AI16" s="67"/>
-      <c r="AJ16" s="67"/>
-      <c r="AK16" s="67"/>
-      <c r="AL16" s="67"/>
-      <c r="AM16" s="67"/>
-      <c r="AN16" s="67"/>
-      <c r="AO16" s="67"/>
-      <c r="AP16" s="67"/>
-      <c r="AQ16" s="67"/>
-      <c r="AR16" s="67"/>
-      <c r="AS16" s="67"/>
-      <c r="AT16" s="67"/>
-      <c r="AU16" s="67"/>
-      <c r="AV16" s="67"/>
-      <c r="AW16" s="67"/>
-      <c r="AX16" s="67"/>
-      <c r="AY16" s="67"/>
-      <c r="AZ16" s="67"/>
-      <c r="BA16" s="67"/>
-      <c r="BB16" s="67"/>
-      <c r="BC16" s="67"/>
-      <c r="BD16" s="67"/>
-      <c r="BE16" s="67"/>
-      <c r="BF16" s="67"/>
-      <c r="BG16" s="67"/>
-      <c r="BH16" s="67"/>
-      <c r="BI16" s="67"/>
-      <c r="BJ16" s="67"/>
-      <c r="BK16" s="67"/>
-      <c r="BL16" s="67"/>
-    </row>
-    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="65"/>
+      <c r="O16" s="65"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="65"/>
+      <c r="T16" s="65"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="65"/>
+      <c r="AA16" s="65"/>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="65"/>
+      <c r="AD16" s="65"/>
+      <c r="AE16" s="65"/>
+      <c r="AF16" s="65"/>
+      <c r="AG16" s="65"/>
+      <c r="AH16" s="65"/>
+      <c r="AI16" s="65"/>
+      <c r="AJ16" s="65"/>
+      <c r="AK16" s="65"/>
+      <c r="AL16" s="65"/>
+      <c r="AM16" s="65"/>
+      <c r="AN16" s="65"/>
+      <c r="AO16" s="65"/>
+      <c r="AP16" s="65"/>
+      <c r="AQ16" s="65"/>
+      <c r="AR16" s="65"/>
+      <c r="AS16" s="65"/>
+      <c r="AT16" s="65"/>
+      <c r="AU16" s="65"/>
+      <c r="AV16" s="65"/>
+      <c r="AW16" s="65"/>
+      <c r="AX16" s="65"/>
+      <c r="AY16" s="65"/>
+      <c r="AZ16" s="65"/>
+      <c r="BA16" s="65"/>
+      <c r="BB16" s="65"/>
+      <c r="BC16" s="65"/>
+      <c r="BD16" s="65"/>
+      <c r="BE16" s="65"/>
+      <c r="BF16" s="65"/>
+      <c r="BG16" s="65"/>
+      <c r="BH16" s="65"/>
+      <c r="BI16" s="65"/>
+      <c r="BJ16" s="65"/>
+      <c r="BK16" s="65"/>
+      <c r="BL16" s="65"/>
+    </row>
+    <row r="17" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="70">
+      <c r="D17" s="68">
         <v>1</v>
       </c>
-      <c r="E17" s="71">
+      <c r="E17" s="69">
         <v>45992</v>
       </c>
-      <c r="F17" s="71">
-        <f t="shared" ref="F17:F22" si="6">E17+1</f>
+      <c r="F17" s="69">
+        <f>E17+1</f>
         <v>45993</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="51"/>
-      <c r="AC17" s="51"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="51"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="51"/>
-      <c r="AH17" s="51"/>
-      <c r="AI17" s="51"/>
-      <c r="AJ17" s="51"/>
-      <c r="AK17" s="51"/>
-      <c r="AL17" s="51"/>
-      <c r="AM17" s="51"/>
-      <c r="AN17" s="51"/>
-      <c r="AO17" s="51"/>
-      <c r="AP17" s="51"/>
-      <c r="AQ17" s="51"/>
-      <c r="AR17" s="51"/>
-      <c r="AS17" s="51"/>
-      <c r="AT17" s="51"/>
-      <c r="AU17" s="51"/>
-      <c r="AV17" s="51"/>
-      <c r="AW17" s="51"/>
-      <c r="AX17" s="51"/>
-      <c r="AY17" s="51"/>
-      <c r="AZ17" s="51"/>
-      <c r="BA17" s="51"/>
-      <c r="BB17" s="51"/>
-      <c r="BC17" s="51"/>
-      <c r="BD17" s="51"/>
-      <c r="BE17" s="51"/>
-      <c r="BF17" s="51"/>
-      <c r="BG17" s="51"/>
-      <c r="BH17" s="51"/>
-      <c r="BI17" s="51"/>
-      <c r="BJ17" s="51"/>
-      <c r="BK17" s="51"/>
-      <c r="BL17" s="51"/>
-    </row>
-    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="50"/>
+      <c r="AG17" s="50"/>
+      <c r="AH17" s="50"/>
+      <c r="AI17" s="50"/>
+      <c r="AJ17" s="50"/>
+      <c r="AK17" s="50"/>
+      <c r="AL17" s="50"/>
+      <c r="AM17" s="50"/>
+      <c r="AN17" s="50"/>
+      <c r="AO17" s="50"/>
+      <c r="AP17" s="50"/>
+      <c r="AQ17" s="50"/>
+      <c r="AR17" s="50"/>
+      <c r="AS17" s="50"/>
+      <c r="AT17" s="50"/>
+      <c r="AU17" s="50"/>
+      <c r="AV17" s="50"/>
+      <c r="AW17" s="50"/>
+      <c r="AX17" s="50"/>
+      <c r="AY17" s="50"/>
+      <c r="AZ17" s="50"/>
+      <c r="BA17" s="50"/>
+      <c r="BB17" s="50"/>
+      <c r="BC17" s="50"/>
+      <c r="BD17" s="50"/>
+      <c r="BE17" s="50"/>
+      <c r="BF17" s="50"/>
+      <c r="BG17" s="50"/>
+      <c r="BH17" s="50"/>
+      <c r="BI17" s="50"/>
+      <c r="BJ17" s="50"/>
+      <c r="BK17" s="50"/>
+      <c r="BL17" s="50"/>
+    </row>
+    <row r="18" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="70">
+      <c r="D18" s="68">
         <v>1</v>
       </c>
-      <c r="E18" s="71">
+      <c r="E18" s="69">
         <f>E17</f>
         <v>45992</v>
       </c>
-      <c r="F18" s="71">
-        <f t="shared" si="6"/>
+      <c r="F18" s="69">
+        <f>E18+1</f>
         <v>45993</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="51"/>
-      <c r="Z18" s="51"/>
-      <c r="AA18" s="51"/>
-      <c r="AB18" s="51"/>
-      <c r="AC18" s="51"/>
-      <c r="AD18" s="51"/>
-      <c r="AE18" s="51"/>
-      <c r="AF18" s="51"/>
-      <c r="AG18" s="51"/>
-      <c r="AH18" s="51"/>
-      <c r="AI18" s="51"/>
-      <c r="AJ18" s="51"/>
-      <c r="AK18" s="51"/>
-      <c r="AL18" s="51"/>
-      <c r="AM18" s="51"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="51"/>
-      <c r="AP18" s="51"/>
-      <c r="AQ18" s="51"/>
-      <c r="AR18" s="51"/>
-      <c r="AS18" s="51"/>
-      <c r="AT18" s="51"/>
-      <c r="AU18" s="51"/>
-      <c r="AV18" s="51"/>
-      <c r="AW18" s="51"/>
-      <c r="AX18" s="51"/>
-      <c r="AY18" s="51"/>
-      <c r="AZ18" s="51"/>
-      <c r="BA18" s="51"/>
-      <c r="BB18" s="51"/>
-      <c r="BC18" s="51"/>
-      <c r="BD18" s="51"/>
-      <c r="BE18" s="51"/>
-      <c r="BF18" s="51"/>
-      <c r="BG18" s="51"/>
-      <c r="BH18" s="51"/>
-      <c r="BI18" s="51"/>
-      <c r="BJ18" s="51"/>
-      <c r="BK18" s="51"/>
-      <c r="BL18" s="51"/>
-    </row>
-    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
+      <c r="AC18" s="50"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="50"/>
+      <c r="AF18" s="50"/>
+      <c r="AG18" s="50"/>
+      <c r="AH18" s="50"/>
+      <c r="AI18" s="50"/>
+      <c r="AJ18" s="50"/>
+      <c r="AK18" s="50"/>
+      <c r="AL18" s="50"/>
+      <c r="AM18" s="50"/>
+      <c r="AN18" s="50"/>
+      <c r="AO18" s="50"/>
+      <c r="AP18" s="50"/>
+      <c r="AQ18" s="50"/>
+      <c r="AR18" s="50"/>
+      <c r="AS18" s="50"/>
+      <c r="AT18" s="50"/>
+      <c r="AU18" s="50"/>
+      <c r="AV18" s="50"/>
+      <c r="AW18" s="50"/>
+      <c r="AX18" s="50"/>
+      <c r="AY18" s="50"/>
+      <c r="AZ18" s="50"/>
+      <c r="BA18" s="50"/>
+      <c r="BB18" s="50"/>
+      <c r="BC18" s="50"/>
+      <c r="BD18" s="50"/>
+      <c r="BE18" s="50"/>
+      <c r="BF18" s="50"/>
+      <c r="BG18" s="50"/>
+      <c r="BH18" s="50"/>
+      <c r="BI18" s="50"/>
+      <c r="BJ18" s="50"/>
+      <c r="BK18" s="50"/>
+      <c r="BL18" s="50"/>
+    </row>
+    <row r="19" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="70">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="71">
+      <c r="D19" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="69">
         <f>F18</f>
         <v>45993</v>
       </c>
-      <c r="F19" s="71">
-        <f t="shared" si="6"/>
+      <c r="F19" s="69">
+        <f>E19+1</f>
         <v>45994</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
-      <c r="AH19" s="51"/>
-      <c r="AI19" s="51"/>
-      <c r="AJ19" s="51"/>
-      <c r="AK19" s="51"/>
-      <c r="AL19" s="51"/>
-      <c r="AM19" s="51"/>
-      <c r="AN19" s="51"/>
-      <c r="AO19" s="51"/>
-      <c r="AP19" s="51"/>
-      <c r="AQ19" s="51"/>
-      <c r="AR19" s="51"/>
-      <c r="AS19" s="51"/>
-      <c r="AT19" s="51"/>
-      <c r="AU19" s="51"/>
-      <c r="AV19" s="51"/>
-      <c r="AW19" s="51"/>
-      <c r="AX19" s="51"/>
-      <c r="AY19" s="51"/>
-      <c r="AZ19" s="51"/>
-      <c r="BA19" s="51"/>
-      <c r="BB19" s="51"/>
-      <c r="BC19" s="51"/>
-      <c r="BD19" s="51"/>
-      <c r="BE19" s="51"/>
-      <c r="BF19" s="51"/>
-      <c r="BG19" s="51"/>
-      <c r="BH19" s="51"/>
-      <c r="BI19" s="51"/>
-      <c r="BJ19" s="51"/>
-      <c r="BK19" s="51"/>
-      <c r="BL19" s="51"/>
-    </row>
-    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="50"/>
+      <c r="AD19" s="50"/>
+      <c r="AE19" s="50"/>
+      <c r="AF19" s="50"/>
+      <c r="AG19" s="50"/>
+      <c r="AH19" s="50"/>
+      <c r="AI19" s="50"/>
+      <c r="AJ19" s="50"/>
+      <c r="AK19" s="50"/>
+      <c r="AL19" s="50"/>
+      <c r="AM19" s="50"/>
+      <c r="AN19" s="50"/>
+      <c r="AO19" s="50"/>
+      <c r="AP19" s="50"/>
+      <c r="AQ19" s="50"/>
+      <c r="AR19" s="50"/>
+      <c r="AS19" s="50"/>
+      <c r="AT19" s="50"/>
+      <c r="AU19" s="50"/>
+      <c r="AV19" s="50"/>
+      <c r="AW19" s="50"/>
+      <c r="AX19" s="50"/>
+      <c r="AY19" s="50"/>
+      <c r="AZ19" s="50"/>
+      <c r="BA19" s="50"/>
+      <c r="BB19" s="50"/>
+      <c r="BC19" s="50"/>
+      <c r="BD19" s="50"/>
+      <c r="BE19" s="50"/>
+      <c r="BF19" s="50"/>
+      <c r="BG19" s="50"/>
+      <c r="BH19" s="50"/>
+      <c r="BI19" s="50"/>
+      <c r="BJ19" s="50"/>
+      <c r="BK19" s="50"/>
+      <c r="BL19" s="50"/>
+    </row>
+    <row r="20" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="70">
+      <c r="D20" s="68">
         <v>0</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="69">
         <f>E19</f>
         <v>45993</v>
       </c>
-      <c r="F20" s="71">
-        <f t="shared" si="6"/>
+      <c r="F20" s="69">
+        <f>E20+1</f>
         <v>45994</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="51"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="51"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="51"/>
-      <c r="AF20" s="51"/>
-      <c r="AG20" s="51"/>
-      <c r="AH20" s="51"/>
-      <c r="AI20" s="51"/>
-      <c r="AJ20" s="51"/>
-      <c r="AK20" s="51"/>
-      <c r="AL20" s="51"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="51"/>
-      <c r="AO20" s="51"/>
-      <c r="AP20" s="51"/>
-      <c r="AQ20" s="51"/>
-      <c r="AR20" s="51"/>
-      <c r="AS20" s="51"/>
-      <c r="AT20" s="51"/>
-      <c r="AU20" s="51"/>
-      <c r="AV20" s="51"/>
-      <c r="AW20" s="51"/>
-      <c r="AX20" s="51"/>
-      <c r="AY20" s="51"/>
-      <c r="AZ20" s="51"/>
-      <c r="BA20" s="51"/>
-      <c r="BB20" s="51"/>
-      <c r="BC20" s="51"/>
-      <c r="BD20" s="51"/>
-      <c r="BE20" s="51"/>
-      <c r="BF20" s="51"/>
-      <c r="BG20" s="51"/>
-      <c r="BH20" s="51"/>
-      <c r="BI20" s="51"/>
-      <c r="BJ20" s="51"/>
-      <c r="BK20" s="51"/>
-      <c r="BL20" s="51"/>
-    </row>
-    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="50"/>
+      <c r="AD20" s="50"/>
+      <c r="AE20" s="50"/>
+      <c r="AF20" s="50"/>
+      <c r="AG20" s="50"/>
+      <c r="AH20" s="50"/>
+      <c r="AI20" s="50"/>
+      <c r="AJ20" s="50"/>
+      <c r="AK20" s="50"/>
+      <c r="AL20" s="50"/>
+      <c r="AM20" s="50"/>
+      <c r="AN20" s="50"/>
+      <c r="AO20" s="50"/>
+      <c r="AP20" s="50"/>
+      <c r="AQ20" s="50"/>
+      <c r="AR20" s="50"/>
+      <c r="AS20" s="50"/>
+      <c r="AT20" s="50"/>
+      <c r="AU20" s="50"/>
+      <c r="AV20" s="50"/>
+      <c r="AW20" s="50"/>
+      <c r="AX20" s="50"/>
+      <c r="AY20" s="50"/>
+      <c r="AZ20" s="50"/>
+      <c r="BA20" s="50"/>
+      <c r="BB20" s="50"/>
+      <c r="BC20" s="50"/>
+      <c r="BD20" s="50"/>
+      <c r="BE20" s="50"/>
+      <c r="BF20" s="50"/>
+      <c r="BG20" s="50"/>
+      <c r="BH20" s="50"/>
+      <c r="BI20" s="50"/>
+      <c r="BJ20" s="50"/>
+      <c r="BK20" s="50"/>
+      <c r="BL20" s="50"/>
+    </row>
+    <row r="21" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="68">
         <v>0</v>
       </c>
-      <c r="E21" s="71">
+      <c r="E21" s="69">
         <f>F20</f>
         <v>45994</v>
       </c>
-      <c r="F21" s="71">
-        <f t="shared" si="6"/>
+      <c r="F21" s="69">
+        <f>E21+1</f>
         <v>45995</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="I21" s="96"/>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="96"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="96"/>
-      <c r="W21" s="96"/>
-      <c r="X21" s="96"/>
-      <c r="Y21" s="96"/>
-      <c r="Z21" s="96"/>
-      <c r="AA21" s="96"/>
-      <c r="AB21" s="96"/>
-      <c r="AC21" s="96"/>
-      <c r="AD21" s="96"/>
-      <c r="AE21" s="96"/>
-      <c r="AF21" s="96"/>
-      <c r="AG21" s="96"/>
-      <c r="AH21" s="96"/>
-      <c r="AI21" s="96"/>
-      <c r="AJ21" s="96"/>
-      <c r="AK21" s="96"/>
-      <c r="AL21" s="96"/>
-      <c r="AM21" s="96"/>
-      <c r="AN21" s="96"/>
-      <c r="AO21" s="96"/>
-      <c r="AP21" s="96"/>
-      <c r="AQ21" s="96"/>
-      <c r="AR21" s="96"/>
-      <c r="AS21" s="96"/>
-      <c r="AT21" s="96"/>
-      <c r="AU21" s="96"/>
-      <c r="AV21" s="96"/>
-      <c r="AW21" s="96"/>
-      <c r="AX21" s="96"/>
-      <c r="AY21" s="96"/>
-      <c r="AZ21" s="96"/>
-      <c r="BA21" s="96"/>
-      <c r="BB21" s="96"/>
-      <c r="BC21" s="96"/>
-      <c r="BD21" s="96"/>
-      <c r="BE21" s="96"/>
-      <c r="BF21" s="96"/>
-      <c r="BG21" s="96"/>
-      <c r="BH21" s="96"/>
-      <c r="BI21" s="96"/>
-      <c r="BJ21" s="96"/>
-      <c r="BK21" s="96"/>
-      <c r="BL21" s="96"/>
-    </row>
-    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
+      <c r="T21" s="111"/>
+      <c r="U21" s="111"/>
+      <c r="V21" s="111"/>
+      <c r="W21" s="111"/>
+      <c r="X21" s="111"/>
+      <c r="Y21" s="111"/>
+      <c r="Z21" s="111"/>
+      <c r="AA21" s="111"/>
+      <c r="AB21" s="111"/>
+      <c r="AC21" s="111"/>
+      <c r="AD21" s="111"/>
+      <c r="AE21" s="111"/>
+      <c r="AF21" s="111"/>
+      <c r="AG21" s="111"/>
+      <c r="AH21" s="111"/>
+      <c r="AI21" s="111"/>
+      <c r="AJ21" s="111"/>
+      <c r="AK21" s="111"/>
+      <c r="AL21" s="111"/>
+      <c r="AM21" s="111"/>
+      <c r="AN21" s="111"/>
+      <c r="AO21" s="111"/>
+      <c r="AP21" s="111"/>
+      <c r="AQ21" s="111"/>
+      <c r="AR21" s="111"/>
+      <c r="AS21" s="111"/>
+      <c r="AT21" s="111"/>
+      <c r="AU21" s="111"/>
+      <c r="AV21" s="111"/>
+      <c r="AW21" s="111"/>
+      <c r="AX21" s="111"/>
+      <c r="AY21" s="111"/>
+      <c r="AZ21" s="111"/>
+      <c r="BA21" s="111"/>
+      <c r="BB21" s="111"/>
+      <c r="BC21" s="111"/>
+      <c r="BD21" s="111"/>
+      <c r="BE21" s="111"/>
+      <c r="BF21" s="111"/>
+      <c r="BG21" s="111"/>
+      <c r="BH21" s="111"/>
+      <c r="BI21" s="111"/>
+      <c r="BJ21" s="111"/>
+      <c r="BK21" s="111"/>
+      <c r="BL21" s="111"/>
+      <c r="BM21" s="112"/>
+    </row>
+    <row r="22" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="94">
+      <c r="D22" s="106">
         <v>0.8</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E22" s="107">
         <v>45994</v>
       </c>
-      <c r="F22" s="95">
-        <f t="shared" si="6"/>
+      <c r="F22" s="107">
+        <f>E22+1</f>
         <v>45995</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
-      <c r="AH22" s="51"/>
-      <c r="AI22" s="51"/>
-      <c r="AJ22" s="51"/>
-      <c r="AK22" s="51"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="51"/>
-      <c r="AR22" s="51"/>
-      <c r="AS22" s="51"/>
-      <c r="AT22" s="51"/>
-      <c r="AU22" s="51"/>
-      <c r="AV22" s="51"/>
-      <c r="AW22" s="51"/>
-      <c r="AX22" s="51"/>
-      <c r="AY22" s="51"/>
-      <c r="AZ22" s="51"/>
-      <c r="BA22" s="51"/>
-      <c r="BB22" s="51"/>
-      <c r="BC22" s="51"/>
-      <c r="BD22" s="51"/>
-      <c r="BE22" s="51"/>
-      <c r="BF22" s="51"/>
-      <c r="BG22" s="51"/>
-      <c r="BH22" s="51"/>
-      <c r="BI22" s="51"/>
-      <c r="BJ22" s="51"/>
-      <c r="BK22" s="51"/>
-      <c r="BL22" s="51"/>
-    </row>
-    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="109"/>
+      <c r="N22" s="109"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="109"/>
+      <c r="Q22" s="109"/>
+      <c r="R22" s="109"/>
+      <c r="S22" s="109"/>
+      <c r="T22" s="109"/>
+      <c r="U22" s="109"/>
+      <c r="V22" s="109"/>
+      <c r="W22" s="109"/>
+      <c r="X22" s="109"/>
+      <c r="Y22" s="109"/>
+      <c r="Z22" s="109"/>
+      <c r="AA22" s="109"/>
+      <c r="AB22" s="109"/>
+      <c r="AC22" s="109"/>
+      <c r="AD22" s="109"/>
+      <c r="AE22" s="109"/>
+      <c r="AF22" s="109"/>
+      <c r="AG22" s="109"/>
+      <c r="AH22" s="109"/>
+      <c r="AI22" s="109"/>
+      <c r="AJ22" s="109"/>
+      <c r="AK22" s="109"/>
+      <c r="AL22" s="109"/>
+      <c r="AM22" s="109"/>
+      <c r="AN22" s="109"/>
+      <c r="AO22" s="109"/>
+      <c r="AP22" s="109"/>
+      <c r="AQ22" s="109"/>
+      <c r="AR22" s="109"/>
+      <c r="AS22" s="109"/>
+      <c r="AT22" s="109"/>
+      <c r="AU22" s="109"/>
+      <c r="AV22" s="109"/>
+      <c r="AW22" s="109"/>
+      <c r="AX22" s="109"/>
+      <c r="AY22" s="109"/>
+      <c r="AZ22" s="109"/>
+      <c r="BA22" s="109"/>
+      <c r="BB22" s="109"/>
+      <c r="BC22" s="109"/>
+      <c r="BD22" s="109"/>
+      <c r="BE22" s="109"/>
+      <c r="BF22" s="109"/>
+      <c r="BG22" s="109"/>
+      <c r="BH22" s="109"/>
+      <c r="BI22" s="109"/>
+      <c r="BJ22" s="109"/>
+      <c r="BK22" s="109"/>
+      <c r="BL22" s="109"/>
+    </row>
+    <row r="23" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="17"/>
       <c r="H23" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="110"/>
+      <c r="L23" s="110"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="110"/>
+      <c r="U23" s="110"/>
+      <c r="V23" s="110"/>
+      <c r="W23" s="110"/>
+      <c r="X23" s="110"/>
+      <c r="Y23" s="110"/>
+      <c r="Z23" s="110"/>
+      <c r="AA23" s="110"/>
+      <c r="AB23" s="110"/>
+      <c r="AC23" s="110"/>
+      <c r="AD23" s="110"/>
+      <c r="AE23" s="110"/>
+      <c r="AF23" s="110"/>
+      <c r="AG23" s="110"/>
+      <c r="AH23" s="110"/>
+      <c r="AI23" s="110"/>
+      <c r="AJ23" s="110"/>
+      <c r="AK23" s="110"/>
+      <c r="AL23" s="110"/>
+      <c r="AM23" s="110"/>
+      <c r="AN23" s="110"/>
+      <c r="AO23" s="110"/>
+      <c r="AP23" s="110"/>
+      <c r="AQ23" s="110"/>
+      <c r="AR23" s="110"/>
+      <c r="AS23" s="110"/>
+      <c r="AT23" s="110"/>
+      <c r="AU23" s="110"/>
+      <c r="AV23" s="110"/>
+      <c r="AW23" s="110"/>
+      <c r="AX23" s="110"/>
+      <c r="AY23" s="110"/>
+      <c r="AZ23" s="110"/>
+      <c r="BA23" s="110"/>
+      <c r="BB23" s="110"/>
+      <c r="BC23" s="110"/>
+      <c r="BD23" s="110"/>
+      <c r="BE23" s="110"/>
+      <c r="BF23" s="110"/>
+      <c r="BG23" s="110"/>
+      <c r="BH23" s="110"/>
+      <c r="BI23" s="110"/>
+      <c r="BJ23" s="110"/>
+      <c r="BK23" s="110"/>
+      <c r="BL23" s="110"/>
+    </row>
+    <row r="24" spans="1:65" s="45" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="80"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="78"/>
       <c r="G24" s="17"/>
       <c r="H24" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="I24" s="81"/>
-      <c r="J24" s="81"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="81"/>
-      <c r="O24" s="81"/>
-      <c r="P24" s="81"/>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="81"/>
-      <c r="S24" s="81"/>
-      <c r="T24" s="81"/>
-      <c r="U24" s="81"/>
-      <c r="V24" s="81"/>
-      <c r="W24" s="81"/>
-      <c r="X24" s="81"/>
-      <c r="Y24" s="81"/>
-      <c r="Z24" s="81"/>
-      <c r="AA24" s="81"/>
-      <c r="AB24" s="81"/>
-      <c r="AC24" s="81"/>
-      <c r="AD24" s="81"/>
-      <c r="AE24" s="81"/>
-      <c r="AF24" s="81"/>
-      <c r="AG24" s="81"/>
-      <c r="AH24" s="81"/>
-      <c r="AI24" s="81"/>
-      <c r="AJ24" s="81"/>
-      <c r="AK24" s="81"/>
-      <c r="AL24" s="81"/>
-      <c r="AM24" s="81"/>
-      <c r="AN24" s="81"/>
-      <c r="AO24" s="81"/>
-      <c r="AP24" s="81"/>
-      <c r="AQ24" s="81"/>
-      <c r="AR24" s="81"/>
-      <c r="AS24" s="81"/>
-      <c r="AT24" s="81"/>
-      <c r="AU24" s="81"/>
-      <c r="AV24" s="81"/>
-      <c r="AW24" s="81"/>
-      <c r="AX24" s="81"/>
-      <c r="AY24" s="81"/>
-      <c r="AZ24" s="81"/>
-      <c r="BA24" s="81"/>
-      <c r="BB24" s="81"/>
-      <c r="BC24" s="81"/>
-      <c r="BD24" s="81"/>
-      <c r="BE24" s="81"/>
-      <c r="BF24" s="81"/>
-      <c r="BG24" s="81"/>
-      <c r="BH24" s="81"/>
-      <c r="BI24" s="81"/>
-      <c r="BJ24" s="81"/>
-      <c r="BK24" s="81"/>
-      <c r="BL24" s="81"/>
-    </row>
-    <row r="25" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="79"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="79"/>
+      <c r="Y24" s="79"/>
+      <c r="Z24" s="79"/>
+      <c r="AA24" s="79"/>
+      <c r="AB24" s="79"/>
+      <c r="AC24" s="79"/>
+      <c r="AD24" s="79"/>
+      <c r="AE24" s="79"/>
+      <c r="AF24" s="79"/>
+      <c r="AG24" s="79"/>
+      <c r="AH24" s="79"/>
+      <c r="AI24" s="79"/>
+      <c r="AJ24" s="79"/>
+      <c r="AK24" s="79"/>
+      <c r="AL24" s="79"/>
+      <c r="AM24" s="79"/>
+      <c r="AN24" s="79"/>
+      <c r="AO24" s="79"/>
+      <c r="AP24" s="79"/>
+      <c r="AQ24" s="79"/>
+      <c r="AR24" s="79"/>
+      <c r="AS24" s="79"/>
+      <c r="AT24" s="79"/>
+      <c r="AU24" s="79"/>
+      <c r="AV24" s="79"/>
+      <c r="AW24" s="79"/>
+      <c r="AX24" s="79"/>
+      <c r="AY24" s="79"/>
+      <c r="AZ24" s="79"/>
+      <c r="BA24" s="79"/>
+      <c r="BB24" s="79"/>
+      <c r="BC24" s="79"/>
+      <c r="BD24" s="79"/>
+      <c r="BE24" s="79"/>
+      <c r="BF24" s="79"/>
+      <c r="BG24" s="79"/>
+      <c r="BH24" s="79"/>
+      <c r="BI24" s="79"/>
+      <c r="BJ24" s="79"/>
+      <c r="BK24" s="79"/>
+      <c r="BL24" s="79"/>
+    </row>
+    <row r="25" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C26" s="16"/>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C27" s="4"/>
     </row>
   </sheetData>
@@ -3743,111 +3839,111 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.94921875" defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="87" style="7" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="87.0390625" style="7" customWidth="1"/>
+    <col min="2" max="16384" width="8.94921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:2" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2" s="85" t="s">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="83" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="86"/>
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="84"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="1.1000000000000001">
-      <c r="A4" s="87" t="s">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="88" t="s">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="86" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="85" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="89" t="s">
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="87" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="1.1000000000000001">
-      <c r="A8" s="87" t="s">
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="85" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="88" t="s">
+    <row r="9" spans="1:2" ht="39" x14ac:dyDescent="0.15">
+      <c r="A9" s="86" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="90" t="s">
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="88" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="1.1000000000000001">
-      <c r="A11" s="87" t="s">
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="85" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="27" x14ac:dyDescent="0.35">
-      <c r="A12" s="88" t="s">
+    <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="86" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="90" t="s">
+    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="88" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="1.1000000000000001">
-      <c r="A14" s="87" t="s">
+    <row r="14" spans="1:2" s="10" customFormat="1" ht="30.75" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="85" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="88" t="s">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="86" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="88" t="s">
+    <row r="16" spans="1:2" ht="63.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="91"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="91"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="91"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="91"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="91"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="91"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="91"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="91"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="89"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="89"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="89"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="89"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="89"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="89"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="89"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="89"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3862,26 +3958,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4193,7 +4269,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4202,47 +4278,42 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A09426A3-87E9-4865-8A6C-3456B026AE03}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4250,6 +4321,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>